<commit_message>
bijgewerkte akties en Arduino libraries
</commit_message>
<xml_diff>
--- a/Akties Ontwortelde boom.xlsx
+++ b/Akties Ontwortelde boom.xlsx
@@ -135,10 +135,23 @@
     <t>Waar komt foutmelding "****file bestaat niet meer" vandaan? Te volle SD kaart?</t>
   </si>
   <si>
-    <t>BT snelheid in Frankrijk aanpassen aan 19200</t>
-  </si>
-  <si>
     <t>WIFI of internetaansluiting mogelijk?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BT snelheid in Frankrijk aanpassen aan 19200. 10-2-2016: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lukt niet.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -189,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -205,6 +218,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +522,9 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -556,7 +574,9 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="7">
+        <v>42410</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -679,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -862,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6">

</xml_diff>